<commit_message>
Raaputin nyt ilmoittaa matkan keston muodossa HH:MM. Lipun hinnan vaihto aloitettu, riippuen alennusryhmasta. Myos Tyotuntejakirjattu.
</commit_message>
<xml_diff>
--- a/TyoTunnit/Juuso.xlsx
+++ b/TyoTunnit/Juuso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>PVM</t>
   </si>
@@ -36,13 +36,19 @@
     <t>jossakkii</t>
   </si>
   <si>
-    <t>3 tai 4</t>
-  </si>
-  <si>
     <t>Tapaamiset</t>
   </si>
   <si>
     <t>Kotona</t>
+  </si>
+  <si>
+    <t>12-14.4</t>
+  </si>
+  <si>
+    <t>Tutkiskelin omaa koodiani ja opettelin pythonia</t>
+  </si>
+  <si>
+    <t>tapaaminen ja lisäkoodausta</t>
   </si>
 </sst>
 </file>
@@ -78,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +417,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -421,7 +428,7 @@
       <c r="A3" s="1">
         <v>41366</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>6</v>
       </c>
       <c r="C3" t="s">
@@ -432,37 +439,138 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41374</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>41379</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tyotunteja ja listan testausta
</commit_message>
<xml_diff>
--- a/TyoTunnit/Juuso.xlsx
+++ b/TyoTunnit/Juuso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>PVM</t>
   </si>
@@ -27,9 +27,6 @@
     <t>LISÄTIEDOT</t>
   </si>
   <si>
-    <t>26.3?</t>
-  </si>
-  <si>
     <t>projektihuoneella</t>
   </si>
   <si>
@@ -55,6 +52,15 @@
   </si>
   <si>
     <t>24-30.4</t>
+  </si>
+  <si>
+    <t>6 - 12 toukokuuta</t>
+  </si>
+  <si>
+    <t>26.3? + -</t>
+  </si>
+  <si>
+    <t>koodin ja MHn sivujen tutkimista kotona + pikkusen ehkä bootstrappia</t>
   </si>
 </sst>
 </file>
@@ -90,10 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +405,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,13 +428,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -438,29 +445,29 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,18 +478,18 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -493,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -515,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -526,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,18 +544,18 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -559,14 +566,30 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
+      <c r="A16" s="1">
+        <v>41407</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>

</xml_diff>

<commit_message>
hinnan laskua lisatty, ja suositellun paikan valinta. + tunteja
</commit_message>
<xml_diff>
--- a/TyoTunnit/Juuso.xlsx
+++ b/TyoTunnit/Juuso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>PVM</t>
   </si>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,52 +591,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41408</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
raaputin viimeistelty + tyotunnit lisatty
</commit_message>
<xml_diff>
--- a/TyoTunnit/Juuso.xlsx
+++ b/TyoTunnit/Juuso.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Taul2" sheetId="2" r:id="rId2"/>
     <sheet name="Taul3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>PVM</t>
   </si>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,15 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+      <c r="A18" s="1">
+        <v>41409</v>
+      </c>
+      <c r="B18" s="2">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -630,7 +638,10 @@
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="B27" s="2">
+        <f>SUM(B2:B26)</f>
+        <v>92</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>

</xml_diff>